<commit_message>
testing all the spreadsheets now
</commit_message>
<xml_diff>
--- a/pkg/datamaps/testdata/test_template.xlsx
+++ b/pkg/datamaps/testdata/test_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date:</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">botticelli</t>
   </si>
   <si>
+    <t xml:space="preserve">Rabbit Helga</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Department</t>
   </si>
   <si>
@@ -60,7 +63,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -153,7 +156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -163,7 +166,7 @@
       <selection pane="topLeft" activeCell="IG10" activeCellId="0" sqref="IG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -288,7 +291,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="IG10" s="0" t="s">
+      <c r="IG10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -304,17 +307,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N39"/>
+  <dimension ref="A3:DI39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="DI15" activeCellId="0" sqref="DI15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -886,6 +889,9 @@
       </c>
       <c r="N15" s="2" t="n">
         <v>43767</v>
+      </c>
+      <c r="DI15" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,37 +1962,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J9" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
-        <v>9</v>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests passing but only with the help of a hack to solve DD/MM/YY
</commit_message>
<xml_diff>
--- a/pkg/datamaps/testdata/test_template.xlsx
+++ b/pkg/datamaps/testdata/test_template.xlsx
@@ -166,7 +166,7 @@
       <selection pane="topLeft" activeCell="IG10" activeCellId="0" sqref="IG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -313,11 +313,11 @@
   </sheetPr>
   <dimension ref="A3:DI39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DI15" activeCellId="0" sqref="DI15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -336,7 +336,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>43760</v>
+        <v>43759</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
@@ -890,7 +890,7 @@
       <c r="N15" s="2" t="n">
         <v>43767</v>
       </c>
-      <c r="DI15" s="0" t="s">
+      <c r="DI15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1972,7 +1972,7 @@
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.79"/>
   </cols>

</xml_diff>